<commit_message>
Chuyen Khoa ProfileID tu int sang string Guid
</commit_message>
<xml_diff>
--- a/BTS.Web/AppFiles/Samples/Import BTS Certificate Sample.xlsx
+++ b/BTS.Web/AppFiles/Samples/Import BTS Certificate Sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="14805" windowHeight="7875" tabRatio="581" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="14805" windowHeight="7875" tabRatio="581" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="InCaseOf" sheetId="11" r:id="rId1"/>
@@ -1012,9 +1012,6 @@
     <t>Bình Phước</t>
   </si>
   <si>
-    <t>BRV</t>
-  </si>
-  <si>
     <t>Bà Rịa - Vũng Tàu</t>
   </si>
   <si>
@@ -1024,9 +1021,6 @@
     <t>Bình Thuận</t>
   </si>
   <si>
-    <t>BTR</t>
-  </si>
-  <si>
     <t>Bến Tre</t>
   </si>
   <si>
@@ -1364,6 +1358,12 @@
   </si>
   <si>
     <t>SharedAntens</t>
+  </si>
+  <si>
+    <t>BTE</t>
+  </si>
+  <si>
+    <t>VTU</t>
   </si>
 </sst>
 </file>
@@ -3373,7 +3373,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3384,7 +3384,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3395,7 +3395,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3406,7 +3406,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -3462,19 +3462,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -3491,8 +3491,8 @@
   </sheetPr>
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3562,10 +3562,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3573,10 +3573,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -3584,10 +3584,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>39</v>
+        <v>151</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -3595,7 +3595,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>4</v>
@@ -3606,10 +3606,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -3617,10 +3617,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -3628,10 +3628,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -3642,7 +3642,7 @@
         <v>27</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -3650,7 +3650,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>1</v>
@@ -3661,7 +3661,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>5</v>
@@ -3672,10 +3672,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -3683,10 +3683,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -3694,10 +3694,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -3705,7 +3705,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>2</v>
@@ -3716,10 +3716,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -3727,10 +3727,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -3738,10 +3738,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -3749,10 +3749,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -3798,7 +3798,7 @@
         <v>23</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3809,7 +3809,7 @@
         <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3820,7 +3820,7 @@
         <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3831,7 +3831,7 @@
         <v>22</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3839,10 +3839,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -3895,7 +3895,7 @@
         <v>9</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>11</v>
@@ -3906,25 +3906,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="E2" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>148</v>
-      </c>
       <c r="H2" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3960,7 +3960,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>13</v>
@@ -3969,7 +3969,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>14</v>
@@ -3989,10 +3989,10 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C2" s="11">
         <v>42962</v>
@@ -4007,7 +4007,7 @@
         <v>10000000</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H2" s="11">
         <v>42964</v>
@@ -4030,7 +4030,7 @@
   </sheetPr>
   <dimension ref="A1:J406"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -4052,13 +4052,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>25</v>
@@ -4067,7 +4067,7 @@
         <v>26</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H1" s="31"/>
       <c r="I1" s="31"/>
@@ -4081,7 +4081,7 @@
         <v>359018</v>
       </c>
       <c r="C2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D2" t="s">
         <v>27</v>
@@ -4104,7 +4104,7 @@
         <v>359184</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D3" t="s">
         <v>27</v>
@@ -4127,7 +4127,7 @@
         <v>359356</v>
       </c>
       <c r="C4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D4" t="s">
         <v>27</v>
@@ -4150,7 +4150,7 @@
         <v>359389</v>
       </c>
       <c r="C5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D5" t="s">
         <v>27</v>
@@ -5831,7 +5831,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E1" s="24" t="s">
         <v>25</v>
@@ -5840,70 +5840,70 @@
         <v>26</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H1" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="K1" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="M1" s="24" t="s">
         <v>73</v>
-      </c>
-      <c r="K1" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="L1" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="M1" s="24" t="s">
-        <v>75</v>
       </c>
       <c r="N1" s="24" t="s">
         <v>24</v>
       </c>
       <c r="O1" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="P1" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q1" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="R1" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="Q1" s="27" t="s">
+      <c r="S1" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="T1" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="R1" s="28" t="s">
+      <c r="U1" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="S1" s="28" t="s">
-        <v>152</v>
-      </c>
-      <c r="T1" s="28" t="s">
+      <c r="V1" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="U1" s="28" t="s">
+      <c r="W1" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="V1" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="W1" s="28" t="s">
-        <v>105</v>
-      </c>
       <c r="X1" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y1" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z1" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="Y1" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z1" s="28" t="s">
-        <v>78</v>
-      </c>
       <c r="AA1" s="28" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="AB1" s="28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:28" ht="15">
@@ -5914,31 +5914,31 @@
         <v>359018</v>
       </c>
       <c r="C2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
         <v>27</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J2" s="11">
         <v>42976</v>
       </c>
       <c r="K2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L2" s="11">
         <f>DATE(MID(K2,11,2)+2000,MID(K2,9,2),MID(K2,7,2))</f>
@@ -5952,31 +5952,31 @@
         <v>2</v>
       </c>
       <c r="O2" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="P2" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>117</v>
+      </c>
+      <c r="R2" t="s">
         <v>118</v>
-      </c>
-      <c r="P2" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R2" t="s">
-        <v>120</v>
       </c>
       <c r="S2">
         <v>0</v>
       </c>
       <c r="T2" t="s">
+        <v>119</v>
+      </c>
+      <c r="U2" t="s">
+        <v>120</v>
+      </c>
+      <c r="V2" t="s">
         <v>121</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>122</v>
-      </c>
-      <c r="V2" t="s">
-        <v>123</v>
-      </c>
-      <c r="W2" t="s">
-        <v>124</v>
       </c>
       <c r="X2">
         <v>29</v>
@@ -6001,7 +6001,7 @@
         <v>359184</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D3" t="s">
         <v>27</v>
@@ -6010,22 +6010,22 @@
         <v>106.6932</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J3" s="11">
         <v>42976</v>
       </c>
       <c r="K3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L3" s="11">
         <f>DATE(MID(K3,11,2)+2000,MID(K3,9,2),MID(K3,7,2))</f>
@@ -6039,31 +6039,31 @@
         <v>2</v>
       </c>
       <c r="O3" s="35" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="P3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="Q3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="R3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="S3">
         <v>0</v>
       </c>
       <c r="T3" t="s">
+        <v>127</v>
+      </c>
+      <c r="U3" t="s">
+        <v>128</v>
+      </c>
+      <c r="V3" t="s">
+        <v>121</v>
+      </c>
+      <c r="W3" t="s">
         <v>129</v>
-      </c>
-      <c r="U3" t="s">
-        <v>130</v>
-      </c>
-      <c r="V3" t="s">
-        <v>123</v>
-      </c>
-      <c r="W3" t="s">
-        <v>131</v>
       </c>
       <c r="X3">
         <v>20</v>
@@ -6088,31 +6088,31 @@
         <v>359356</v>
       </c>
       <c r="C4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D4" t="s">
         <v>27</v>
       </c>
       <c r="E4" s="34" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J4" s="11">
         <v>42976</v>
       </c>
       <c r="K4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L4" s="11">
         <f>DATE(MID(K4,11,2)+2000,MID(K4,9,2),MID(K4,7,2))</f>
@@ -6126,31 +6126,31 @@
         <v>2</v>
       </c>
       <c r="O4" s="35" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="P4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="Q4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="R4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="S4">
         <v>0</v>
       </c>
       <c r="T4" t="s">
+        <v>135</v>
+      </c>
+      <c r="U4" t="s">
+        <v>136</v>
+      </c>
+      <c r="V4" t="s">
+        <v>121</v>
+      </c>
+      <c r="W4" t="s">
         <v>137</v>
-      </c>
-      <c r="U4" t="s">
-        <v>138</v>
-      </c>
-      <c r="V4" t="s">
-        <v>123</v>
-      </c>
-      <c r="W4" t="s">
-        <v>139</v>
       </c>
       <c r="X4">
         <v>20</v>
@@ -9310,7 +9310,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E1" s="24" t="s">
         <v>25</v>
@@ -9319,19 +9319,19 @@
         <v>26</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H1" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="J1" s="24" t="s">
-        <v>73</v>
-      </c>
       <c r="K1" s="24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15">
@@ -9342,31 +9342,31 @@
         <v>359389</v>
       </c>
       <c r="C2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D2" t="s">
         <v>27</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J2" s="11">
         <v>42976</v>
       </c>
       <c r="K2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:11">

</xml_diff>

<commit_message>
Modify to support the new ImportData Sample File
</commit_message>
<xml_diff>
--- a/BTS.Web/AppFiles/Samples/Import BTS Certificate Sample.xlsx
+++ b/BTS.Web/AppFiles/Samples/Import BTS Certificate Sample.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\BTS\BTS.Web\AppFiles\Samples\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="14805" windowHeight="7875" tabRatio="581" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="14805" windowHeight="7875" tabRatio="581" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="InCaseOf" sheetId="11" r:id="rId1"/>
@@ -33,7 +38,7 @@
     <definedName name="NV">[3]Drawing!$ED$1:$EL$1</definedName>
     <definedName name="Operators">Operator!$A$1:$C$6</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -43,7 +48,7 @@
     <author>Dell</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -68,7 +73,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +107,7 @@
     <author>Dell</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -127,7 +132,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -151,7 +156,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -175,7 +180,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -199,7 +204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -233,7 +238,7 @@
     <author>Dell</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -258,7 +263,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -292,7 +297,7 @@
     <author>Dell</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -317,7 +322,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -351,7 +356,7 @@
     <author>Dell</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -376,7 +381,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -400,7 +405,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -424,7 +429,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -448,7 +453,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -472,7 +477,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -496,7 +501,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -516,21 +521,11 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-- Mã nhà mạng phải thuộc trong danh sách Mã nhà mạng thuộc Sheet Operator đã khai báo.</t>
+- Tên nhà mạng phải thuộc trong danh sách nhà mạng thuộc Sheet Operator đã khai báo.</t>
         </r>
       </text>
     </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Dell</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -550,11 +545,69 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-- Mã đơn vị không quá 50 ký tự.</t>
+- Mã nhà mạng (Optional) phải thuộc trong danh sách Mã nhà mạng thuộc Sheet Operator đã khai báo.</t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Dell</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- Mã đơn vị (Optional) phải thuộc trong danh sách Đơn vị thuộc Sheet Applicant đã khai báo.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- Tên đơn vị không quá 255 ký tự phải thuộc trong danh sách Đơn vị thuộc Sheet Applicant đã khai báo.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -578,7 +631,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -602,7 +655,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -622,11 +675,35 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-- Số Trạm BTS KĐ: Số nguyên.</t>
+- Số Trạm BTS KĐ theo đơn: Số nguyên.</t>
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- Số Trạm BTS KĐ được tiếp nhận: Số nguyên.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -650,7 +727,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -674,7 +751,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -698,7 +775,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -722,7 +799,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -756,7 +833,7 @@
     <author>Dell</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -780,7 +857,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -804,7 +881,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -828,7 +905,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -852,7 +929,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -876,7 +953,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -905,7 +982,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="156">
   <si>
     <t>No</t>
   </si>
@@ -1364,12 +1441,21 @@
   </si>
   <si>
     <t>VTU</t>
+  </si>
+  <si>
+    <t>OperatorName</t>
+  </si>
+  <si>
+    <t>ApplicantName</t>
+  </si>
+  <si>
+    <t>AcceptedBtsQuantity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="40">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
@@ -2701,6 +2787,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -3094,7 +3183,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3129,7 +3218,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3338,13 +3427,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet1">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3417,13 +3506,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet2">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3486,13 +3575,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet3">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3763,13 +3852,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet4">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3853,13 +3942,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet5">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3870,12 +3959,12 @@
     <col min="4" max="4" width="30" style="4" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" style="4" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" style="5" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="4"/>
+    <col min="7" max="8" width="17.85546875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1">
+    <row r="1" spans="1:9" s="8" customFormat="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -3898,10 +3987,13 @@
         <v>91</v>
       </c>
       <c r="H1" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9" ht="30">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -3924,8 +4016,9 @@
         <v>146</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>85</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="I2" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3936,83 +4029,95 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet6">
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:11" s="1" customFormat="1">
       <c r="A1" s="9" t="s">
         <v>104</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:11" ht="30">
       <c r="A2" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="11">
+      <c r="D2" s="11">
         <v>42962</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>4</v>
       </c>
-      <c r="E2" s="11">
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2" s="11">
         <v>42963</v>
       </c>
-      <c r="F2" s="13">
+      <c r="H2" s="13">
         <v>10000000</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="I2" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="H2" s="11">
+      <c r="J2" s="11">
         <v>42964</v>
       </c>
-      <c r="I2" s="11">
+      <c r="K2" s="11">
         <v>42972</v>
       </c>
     </row>
@@ -4025,20 +4130,20 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet7">
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A1:J406"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="7.85546875" style="16" customWidth="1"/>
     <col min="2" max="2" width="11.140625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="81.5703125" style="18" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="14" style="18" customWidth="1"/>
     <col min="8" max="10" width="12.140625" style="18" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" style="18" customWidth="1"/>
@@ -5778,13 +5883,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet8">
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A1:AB404"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W4" sqref="W4"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Z1" sqref="Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -5792,7 +5897,7 @@
     <col min="1" max="1" width="3.42578125" style="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" style="26" customWidth="1"/>
     <col min="3" max="3" width="46.140625" style="23" customWidth="1"/>
-    <col min="4" max="4" width="4.85546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="26" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" style="26" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" style="26" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" style="26" customWidth="1"/>
@@ -5816,7 +5921,7 @@
     <col min="25" max="25" width="16.28515625" style="29" customWidth="1"/>
     <col min="26" max="26" width="14.28515625" style="29" customWidth="1"/>
     <col min="27" max="27" width="16.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.28515625" style="29" customWidth="1"/>
+    <col min="28" max="28" width="11.42578125" style="29" customWidth="1"/>
     <col min="29" max="16384" width="9" style="22"/>
   </cols>
   <sheetData>
@@ -9274,7 +9379,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet9">
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A1:K402"/>

</xml_diff>